<commit_message>
Tilføjede emner til tidsplan.
</commit_message>
<xml_diff>
--- a/Tekster/Tidsplan.xlsx
+++ b/Tekster/Tidsplan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Uge:</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Simple problemløsninger</t>
-  </si>
-  <si>
-    <t>Koderi af "lavere klasser"</t>
   </si>
   <si>
     <t>Begynd så småt på tests 
@@ -146,6 +143,21 @@
   </si>
   <si>
     <t>Forelæsning om database</t>
+  </si>
+  <si>
+    <t>Kodning af "lavere klasser"</t>
+  </si>
+  <si>
+    <t>Diskussion af controller-
+implementation</t>
+  </si>
+  <si>
+    <t>Implementation af 
+toString()-metoder i alle klasser</t>
+  </si>
+  <si>
+    <t>Diskussion af GUI-
+mockups</t>
   </si>
 </sst>
 </file>
@@ -536,7 +548,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -681,6 +693,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1031,7 +1046,7 @@
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+      <selection pane="topRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1070,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="16.5">
+    <row r="3" spans="2:18" ht="16">
       <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
@@ -1123,7 +1138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="16.5">
+    <row r="4" spans="2:18" ht="16">
       <c r="B4" s="24"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
@@ -1184,7 +1199,7 @@
       <c r="Q6" s="35"/>
       <c r="R6" s="18"/>
     </row>
-    <row r="7" spans="2:18" ht="16.5">
+    <row r="7" spans="2:18" ht="16">
       <c r="B7" s="25"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -1222,7 +1237,7 @@
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
     </row>
-    <row r="9" spans="2:18" ht="16.5">
+    <row r="9" spans="2:18" ht="16">
       <c r="B9" s="27"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -1241,7 +1256,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
     </row>
-    <row r="10" spans="2:18" ht="16.5">
+    <row r="10" spans="2:18" ht="16">
       <c r="B10" s="27"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -1286,7 +1301,7 @@
     <row r="12" spans="2:18" ht="43" customHeight="1">
       <c r="B12" s="45"/>
       <c r="C12" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>29</v>
@@ -1295,10 +1310,10 @@
         <v>26</v>
       </c>
       <c r="F12" s="49" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G12" s="50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="50"/>
       <c r="I12" s="51"/>
@@ -1321,11 +1336,13 @@
         <v>31</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="49"/>
+        <v>35</v>
+      </c>
+      <c r="F13" s="65" t="s">
+        <v>41</v>
+      </c>
       <c r="G13" s="54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="50"/>
       <c r="I13" s="51"/>
@@ -1350,7 +1367,9 @@
       <c r="E14" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="49"/>
+      <c r="F14" s="65" t="s">
+        <v>42</v>
+      </c>
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
       <c r="I14" s="51"/>
@@ -1371,9 +1390,11 @@
         <v>34</v>
       </c>
       <c r="E15" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="G15" s="50"/>
       <c r="H15" s="50"/>
       <c r="I15" s="51"/>

</xml_diff>

<commit_message>
Rettede tidsplan for dagen.
</commit_message>
<xml_diff>
--- a/Tekster/Tidsplan.xlsx
+++ b/Tekster/Tidsplan.xlsx
@@ -145,19 +145,20 @@
     <t>Forelæsning om database</t>
   </si>
   <si>
-    <t>Kodning af "lavere klasser"</t>
-  </si>
-  <si>
     <t>Diskussion af controller-
 implementation</t>
   </si>
   <si>
-    <t>Implementation af 
-toString()-metoder i alle klasser</t>
-  </si>
-  <si>
     <t>Diskussion af GUI-
 mockups</t>
+  </si>
+  <si>
+    <t>Reservation Hashset/MapSet 
+mellem pers. og sæde</t>
+  </si>
+  <si>
+    <t>Kodning af 
+"lavere klasser"</t>
   </si>
 </sst>
 </file>
@@ -537,10 +538,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -698,14 +711,26 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1046,7 +1071,7 @@
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+      <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1309,7 +1334,7 @@
       <c r="E12" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="65" t="s">
         <v>40</v>
       </c>
       <c r="G12" s="50" t="s">
@@ -1368,7 +1393,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="65" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
@@ -1393,7 +1418,7 @@
         <v>36</v>
       </c>
       <c r="F15" s="65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="50"/>
       <c r="H15" s="50"/>

</xml_diff>